<commit_message>
Inclusão de testes de contratação e cancelamento web
</commit_message>
<xml_diff>
--- a/src/test/resources/armazenador/bloqueioPainel/Desloqueio dentro do periodo de testes.xlsx
+++ b/src/test/resources/armazenador/bloqueioPainel/Desloqueio dentro do periodo de testes.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\git\PortalEC\src\test\resources\armazenador\bloqueioPainel\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\git\PortalEc_Web\src\test\resources\armazenador\bloqueioPainel\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -42,7 +42,7 @@
     <t>Desbloquear</t>
   </si>
   <si>
-    <t>28339982000160</t>
+    <t>41707658000115</t>
   </si>
 </sst>
 </file>

</xml_diff>